<commit_message>
Function to unmerge cells and preserve data works
</commit_message>
<xml_diff>
--- a/data_cleaning/1.test_data/B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/data_cleaning/1.test_data/B0.02 B0.03 B0.04 Timetable.xlsx
@@ -51,59 +51,6 @@
       </text>
     </comment>
     <comment ref="H7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Mollie:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Module did not run in semester 1, awaiting insight as to why module was timetabled from module coordinator. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Mollie:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>COMP30520 = 60
-COMP41110 = 19</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -379,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="78">
   <si>
     <t>B0.02</t>
   </si>
@@ -390,136 +337,136 @@
     <t>Room capacity: 90</t>
   </si>
   <si>
+    <t>Monday 2nd </t>
+  </si>
+  <si>
+    <t>No. of registered students </t>
+  </si>
+  <si>
+    <t>Tuesday 3rd</t>
+  </si>
+  <si>
+    <t>Wednesday 4th </t>
+  </si>
+  <si>
+    <t>Thursday 5th</t>
+  </si>
+  <si>
+    <t>Friday 6th</t>
+  </si>
+  <si>
+    <t>9:00 - 10:00</t>
+  </si>
+  <si>
+    <t>COMP30190</t>
+  </si>
+  <si>
+    <t>COMP30220</t>
+  </si>
+  <si>
+    <t>10:00 - 11:00</t>
+  </si>
+  <si>
+    <t>COMP40660</t>
+  </si>
+  <si>
+    <t>COMP30110</t>
+  </si>
+  <si>
+    <t>11:00 - 12:00</t>
+  </si>
+  <si>
+    <t>COMP30260</t>
+  </si>
+  <si>
+    <t>COMP30250</t>
+  </si>
+  <si>
+    <t>COMP40370</t>
+  </si>
+  <si>
+    <t>12:00 - 13:00</t>
+  </si>
+  <si>
+    <t>COMP41690 (Practical)</t>
+  </si>
+  <si>
+    <t>13:00 - 14:00</t>
+  </si>
+  <si>
+    <t>COMP41690</t>
+  </si>
+  <si>
+    <t>COMP41690 (Lecture)</t>
+  </si>
+  <si>
+    <t>COMP47290</t>
+  </si>
+  <si>
+    <t>COMP30170</t>
+  </si>
+  <si>
+    <t>14:00 - 15:00</t>
+  </si>
+  <si>
+    <t>COMP30240</t>
+  </si>
+  <si>
+    <t>15:00 - 16:00</t>
+  </si>
+  <si>
+    <t>COMP30520 &amp; COMP41110</t>
+  </si>
+  <si>
+    <t>COMP30520</t>
+  </si>
+  <si>
+    <t>16:00 - 17:00</t>
+  </si>
+  <si>
+    <t>17:00 - 18:00</t>
+  </si>
+  <si>
+    <t>B0.03</t>
+  </si>
+  <si>
     <t>9 Nov - 13 Nov</t>
   </si>
   <si>
-    <t>Monday 2nd </t>
-  </si>
-  <si>
-    <t>No. of registered students </t>
-  </si>
-  <si>
-    <t>Tuesday 3rd</t>
-  </si>
-  <si>
-    <t>Wednesday 4th </t>
-  </si>
-  <si>
-    <t>Thursday 5th</t>
-  </si>
-  <si>
-    <t>Friday 6th</t>
-  </si>
-  <si>
-    <t>9:00 - 10:00</t>
-  </si>
-  <si>
-    <t>COMP30190</t>
-  </si>
-  <si>
-    <t>COMP30220</t>
-  </si>
-  <si>
-    <t>10:00 - 11:00</t>
-  </si>
-  <si>
-    <t>COMP40660</t>
-  </si>
-  <si>
-    <t>COMP30110</t>
-  </si>
-  <si>
-    <t>11:00 - 12:00</t>
-  </si>
-  <si>
-    <t>COMP30260</t>
-  </si>
-  <si>
-    <t>COMP30250</t>
-  </si>
-  <si>
-    <t>COMP40370</t>
-  </si>
-  <si>
-    <t>12:00 - 13:00</t>
-  </si>
-  <si>
-    <t>COMP41690 (Practical)</t>
-  </si>
-  <si>
-    <t>13:00 - 14:00</t>
-  </si>
-  <si>
-    <t>COMP41690</t>
-  </si>
-  <si>
-    <t>COMP41690 (Lecture)</t>
-  </si>
-  <si>
-    <t>COMP47290</t>
-  </si>
-  <si>
-    <t>COMP30170</t>
-  </si>
-  <si>
-    <t>14:00 - 15:00</t>
-  </si>
-  <si>
-    <t>COMP30240</t>
-  </si>
-  <si>
-    <t>15:00 - 16:00</t>
-  </si>
-  <si>
-    <t>COMP30520 &amp; COMP41110</t>
-  </si>
-  <si>
-    <t>COMP30520</t>
-  </si>
-  <si>
-    <t>16:00 - 17:00</t>
-  </si>
-  <si>
-    <t>17:00 - 18:00</t>
+    <t>COMP20020</t>
+  </si>
+  <si>
+    <t>COMP47300 (Lecture)</t>
+  </si>
+  <si>
+    <t>COMP30060</t>
+  </si>
+  <si>
+    <t>COMP47300 (Practical)</t>
+  </si>
+  <si>
+    <t>COMP30010</t>
+  </si>
+  <si>
+    <t>COMP10280</t>
+  </si>
+  <si>
+    <t>COMP30080</t>
+  </si>
+  <si>
+    <t>Career opportunities talks</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>COMP47300</t>
   </si>
   <si>
     <t>No class timetabled</t>
   </si>
   <si>
     <t>Unclear if class went ahead</t>
-  </si>
-  <si>
-    <t>B0.03</t>
-  </si>
-  <si>
-    <t>COMP20020</t>
-  </si>
-  <si>
-    <t>COMP47300 (Lecture)</t>
-  </si>
-  <si>
-    <t>COMP30060</t>
-  </si>
-  <si>
-    <t>COMP47300 (Practical)</t>
-  </si>
-  <si>
-    <t>COMP30010</t>
-  </si>
-  <si>
-    <t>COMP10280</t>
-  </si>
-  <si>
-    <t>COMP30080</t>
-  </si>
-  <si>
-    <t>Career opportunities talks</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>COMP47300</t>
   </si>
   <si>
     <t>B0.04</t>
@@ -663,14 +610,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -681,6 +620,14 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1164,7 +1111,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="110">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1333,11 +1280,151 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="32" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1349,7 +1436,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1361,174 +1448,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="32" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1605,19 +1524,19 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1710,10 +1629,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1762,78 +1681,38 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="M1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K2" s="6"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="9" t="n">
         <v>29</v>
@@ -1841,7 +1720,7 @@
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="13" t="n">
         <v>29</v>
@@ -1849,223 +1728,111 @@
       <c r="H3" s="10"/>
       <c r="I3" s="14"/>
       <c r="J3" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K3" s="15" t="n">
         <v>38</v>
       </c>
-      <c r="M3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="9" t="n">
-        <v>29</v>
-      </c>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="S3" s="13" t="n">
-        <v>29</v>
-      </c>
-      <c r="T3" s="10"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="W3" s="15" t="n">
-        <v>38</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>53</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="13" t="n">
         <v>45</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="13" t="n">
         <v>53</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="16" t="n">
         <v>45</v>
       </c>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
-      <c r="M4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="9" t="n">
-        <v>53</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="13" t="n">
-        <v>45</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="S4" s="13" t="n">
-        <v>53</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="U4" s="16" t="n">
-        <v>45</v>
-      </c>
-      <c r="V4" s="17"/>
-      <c r="W4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="19"/>
       <c r="D5" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="13" t="n">
         <v>18</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="13" t="n">
         <v>22</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" s="16" t="n">
         <v>27</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K5" s="21" t="n">
         <v>29</v>
       </c>
-      <c r="M5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q5" s="13" t="n">
-        <v>18</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="S5" s="13" t="n">
-        <v>22</v>
-      </c>
-      <c r="T5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" s="16" t="n">
-        <v>27</v>
-      </c>
-      <c r="V5" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="W5" s="21" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="23" t="n">
         <v>22</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="25" t="n">
         <v>27</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="25" t="n">
         <v>60</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="26" t="n">
         <v>18</v>
       </c>
       <c r="J6" s="20"/>
       <c r="K6" s="21"/>
-      <c r="M6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" s="23" t="n">
-        <v>22</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="25" t="n">
-        <v>27</v>
-      </c>
-      <c r="R6" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="25" t="n">
-        <v>60</v>
-      </c>
-      <c r="T6" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="U6" s="26" t="n">
-        <v>18</v>
-      </c>
-      <c r="V6" s="20"/>
-      <c r="W6" s="21"/>
     </row>
     <row r="7" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="C7" s="9" t="n">
         <v>60</v>
@@ -2073,183 +1840,100 @@
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
       <c r="F7" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="13" t="n">
         <v>60</v>
       </c>
       <c r="H7" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="I7" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="K7" s="15" t="n">
         <v>51</v>
       </c>
-      <c r="M7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" s="9" t="n">
-        <v>60</v>
-      </c>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="S7" s="13" t="n">
-        <v>60</v>
-      </c>
-      <c r="T7" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="U7" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="W7" s="15" t="n">
-        <v>51</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="29" t="n">
         <v>18</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="30" t="n">
         <v>42</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="13" t="n">
         <v>38</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="31" t="n">
         <v>42</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K8" s="16" t="n">
         <v>42</v>
       </c>
-      <c r="M8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" s="29" t="n">
-        <v>18</v>
-      </c>
-      <c r="P8" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q8" s="30" t="n">
-        <v>42</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="S8" s="13" t="n">
-        <v>38</v>
-      </c>
-      <c r="T8" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="U8" s="31" t="n">
-        <v>42</v>
-      </c>
-      <c r="V8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="W8" s="16" t="n">
-        <v>42</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="33"/>
       <c r="D9" s="20"/>
       <c r="E9" s="30"/>
       <c r="F9" s="34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="25" t="n">
         <v>79</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="21" t="n">
         <v>60</v>
       </c>
       <c r="J9" s="36"/>
       <c r="K9" s="37"/>
-      <c r="M9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" s="32"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="S9" s="25" t="n">
-        <v>79</v>
-      </c>
-      <c r="T9" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="U9" s="21" t="n">
-        <v>60</v>
-      </c>
-      <c r="V9" s="36"/>
-      <c r="W9" s="37"/>
     </row>
     <row r="10" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="38" t="n">
         <v>53</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="39" t="n">
         <v>27</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="39" t="n">
         <v>22</v>
@@ -2258,35 +1942,10 @@
       <c r="I10" s="21"/>
       <c r="J10" s="36"/>
       <c r="K10" s="37"/>
-      <c r="M10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" s="38" t="n">
-        <v>53</v>
-      </c>
-      <c r="P10" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="39" t="n">
-        <v>27</v>
-      </c>
-      <c r="R10" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="S10" s="39" t="n">
-        <v>22</v>
-      </c>
-      <c r="T10" s="35"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="36"/>
-      <c r="W10" s="37"/>
     </row>
     <row r="11" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="38"/>
@@ -2298,115 +1957,31 @@
       <c r="I11" s="40"/>
       <c r="J11" s="32"/>
       <c r="K11" s="41"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="20"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="40"/>
-      <c r="V11" s="32"/>
-      <c r="W11" s="41"/>
-    </row>
-    <row r="13" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="45"/>
-    </row>
-    <row r="14" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="48"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="48"/>
-    </row>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="18">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:K1"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="O1:W1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:U10"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="N13:V13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="V14:W14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2459,460 +2034,460 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="50" t="s">
+      <c r="A1" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="M1" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="50" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="M1" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+    </row>
+    <row r="2" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="42"/>
+      <c r="B2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-    </row>
-    <row r="2" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49"/>
-      <c r="B2" s="52" t="s">
+      <c r="C2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="D2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="54"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="52" t="s">
+      <c r="K2" s="47"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="53" t="s">
+      <c r="P2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="54" t="s">
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54" t="s">
+      <c r="S2" s="47"/>
+      <c r="T2" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54" t="s">
+      <c r="U2" s="47"/>
+      <c r="V2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54" t="s">
-        <v>9</v>
-      </c>
-      <c r="W2" s="54"/>
+      <c r="W2" s="47"/>
     </row>
     <row r="3" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="48" t="n">
+        <v>53</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="56" t="n">
+      <c r="I3" s="15" t="n">
+        <v>42</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="52" t="n">
+        <v>45</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="48" t="n">
         <v>53</v>
       </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="59" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="61" t="n">
+      <c r="P3" s="49"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="15" t="n">
         <v>42</v>
       </c>
-      <c r="J3" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="62" t="n">
-        <v>45</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="56" t="n">
-        <v>53</v>
-      </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="59" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="U3" s="61" t="n">
-        <v>42</v>
-      </c>
-      <c r="V3" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" s="62" t="n">
+      <c r="V3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="52" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="62"/>
+        <v>12</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="49"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="52"/>
       <c r="M4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="55"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" s="57"/>
-      <c r="U4" s="67"/>
-      <c r="V4" s="55"/>
-      <c r="W4" s="62"/>
+        <v>12</v>
+      </c>
+      <c r="N4" s="20"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="49"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="52"/>
     </row>
     <row r="5" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="56" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="48" t="n">
         <v>45</v>
       </c>
-      <c r="D5" s="60" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="68" t="n">
+      <c r="D5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="13" t="n">
         <v>56</v>
       </c>
-      <c r="F5" s="65"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="71" t="n">
+      <c r="F5" s="55"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="60" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="O5" s="56" t="n">
+        <v>15</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" s="48" t="n">
         <v>45</v>
       </c>
-      <c r="P5" s="60" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q5" s="68" t="n">
+      <c r="P5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="13" t="n">
         <v>56</v>
       </c>
-      <c r="R5" s="65"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="63"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="70" t="s">
-        <v>25</v>
-      </c>
-      <c r="W5" s="71" t="n">
+      <c r="R5" s="55"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="58"/>
+      <c r="V5" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="W5" s="60" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="72" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="73" t="n">
+        <v>19</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="61" t="n">
         <v>73</v>
       </c>
-      <c r="H6" s="74" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="75" t="n">
+      <c r="H6" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="26" t="n">
         <v>56</v>
       </c>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="60"/>
       <c r="M6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="55"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="64"/>
-      <c r="R6" s="72" t="s">
-        <v>43</v>
-      </c>
-      <c r="S6" s="73" t="n">
+        <v>19</v>
+      </c>
+      <c r="N6" s="20"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="S6" s="61" t="n">
         <v>73</v>
       </c>
-      <c r="T6" s="74" t="s">
-        <v>42</v>
-      </c>
-      <c r="U6" s="75" t="n">
+      <c r="T6" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="U6" s="26" t="n">
         <v>56</v>
       </c>
-      <c r="V6" s="70"/>
-      <c r="W6" s="71"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="60"/>
     </row>
     <row r="7" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="19"/>
-      <c r="D7" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="72"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="77" t="s">
-        <v>45</v>
+      <c r="D7" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="63" t="s">
+        <v>43</v>
       </c>
       <c r="J7" s="17"/>
       <c r="K7" s="14"/>
       <c r="M7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N7" s="17"/>
       <c r="O7" s="19"/>
-      <c r="P7" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="R7" s="72"/>
-      <c r="S7" s="73"/>
-      <c r="T7" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="U7" s="77" t="s">
-        <v>45</v>
+      <c r="P7" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" s="35"/>
+      <c r="S7" s="61"/>
+      <c r="T7" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="U7" s="63" t="s">
+        <v>43</v>
       </c>
       <c r="V7" s="17"/>
       <c r="W7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="64" t="n">
+        <v>33</v>
+      </c>
+      <c r="D8" s="65"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="78" t="n">
+      <c r="K8" s="70" t="n">
+        <v>65</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="64" t="n">
         <v>33</v>
       </c>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="83" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" s="84" t="n">
-        <v>65</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N8" s="55" t="s">
+      <c r="P8" s="65"/>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="S8" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="U8" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="78" t="n">
-        <v>33</v>
-      </c>
-      <c r="P8" s="79"/>
-      <c r="Q8" s="80"/>
-      <c r="R8" s="81" t="s">
-        <v>46</v>
-      </c>
-      <c r="S8" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="U8" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" s="83" t="s">
-        <v>43</v>
-      </c>
-      <c r="W8" s="84" t="n">
+      <c r="W8" s="70" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="66"/>
+        <v>28</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="83"/>
-      <c r="K9" s="84"/>
+        <v>24</v>
+      </c>
+      <c r="I9" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="69"/>
+      <c r="K9" s="70"/>
       <c r="M9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" s="55"/>
-      <c r="O9" s="78"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="86"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="66"/>
+        <v>28</v>
+      </c>
+      <c r="N9" s="20"/>
+      <c r="O9" s="64"/>
+      <c r="P9" s="71"/>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="67"/>
+      <c r="S9" s="56"/>
       <c r="T9" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="U9" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" s="83"/>
-      <c r="W9" s="84"/>
+        <v>24</v>
+      </c>
+      <c r="U9" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" s="69"/>
+      <c r="W9" s="70"/>
     </row>
     <row r="10" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="56" t="n">
+        <v>31</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="48" t="n">
         <v>35</v>
       </c>
-      <c r="D10" s="87"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="89" t="n">
+      <c r="D10" s="73"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="75" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="36"/>
       <c r="K10" s="37"/>
       <c r="M10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="O10" s="56" t="n">
+        <v>31</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="48" t="n">
         <v>35</v>
       </c>
-      <c r="P10" s="87"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="87"/>
-      <c r="S10" s="88"/>
-      <c r="T10" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="U10" s="89" t="n">
+      <c r="P10" s="73"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="U10" s="75" t="n">
         <v>0</v>
       </c>
       <c r="V10" s="36"/>
@@ -2920,78 +2495,78 @@
     </row>
     <row r="11" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="89"/>
+        <v>32</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="75"/>
       <c r="J11" s="32"/>
       <c r="K11" s="41"/>
-      <c r="L11" s="42"/>
+      <c r="L11" s="77"/>
       <c r="M11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="55"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="90"/>
-      <c r="Q11" s="86"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="86"/>
-      <c r="T11" s="81"/>
-      <c r="U11" s="89"/>
+        <v>32</v>
+      </c>
+      <c r="N11" s="20"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="76"/>
+      <c r="Q11" s="72"/>
+      <c r="R11" s="76"/>
+      <c r="S11" s="72"/>
+      <c r="T11" s="67"/>
+      <c r="U11" s="75"/>
       <c r="V11" s="32"/>
       <c r="W11" s="41"/>
     </row>
     <row r="13" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="45"/>
+      <c r="B13" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="80"/>
+      <c r="R13" s="80"/>
+      <c r="S13" s="80"/>
+      <c r="T13" s="80"/>
+      <c r="U13" s="80"/>
+      <c r="V13" s="80"/>
     </row>
     <row r="14" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="48"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="48"/>
+      <c r="B14" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="82"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="83"/>
+      <c r="N14" s="83"/>
+      <c r="O14" s="83"/>
+      <c r="P14" s="83"/>
+      <c r="Q14" s="83"/>
+      <c r="R14" s="83"/>
+      <c r="S14" s="83"/>
+      <c r="T14" s="83"/>
+      <c r="U14" s="83"/>
+      <c r="V14" s="83"/>
+      <c r="W14" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="66">
@@ -3113,611 +2688,611 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="M1" s="91" t="s">
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="M1" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="92" t="s">
+      <c r="N1" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+    </row>
+    <row r="2" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="84"/>
+      <c r="B2" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="93" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93"/>
-      <c r="T1" s="93"/>
-      <c r="U1" s="93"/>
-      <c r="V1" s="93"/>
-      <c r="W1" s="93"/>
-    </row>
-    <row r="2" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="91"/>
-      <c r="B2" s="94" t="s">
+      <c r="C2" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="95" t="s">
+      <c r="D2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="96" t="s">
+      <c r="E2" s="89"/>
+      <c r="F2" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96" t="s">
+      <c r="G2" s="89"/>
+      <c r="H2" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="96"/>
-      <c r="H2" s="97" t="s">
+      <c r="I2" s="90"/>
+      <c r="J2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="97"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="94" t="s">
+      <c r="K2" s="90"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="87" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="95" t="s">
+      <c r="P2" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="96" t="s">
+      <c r="Q2" s="89"/>
+      <c r="R2" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96" t="s">
+      <c r="S2" s="89"/>
+      <c r="T2" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="96"/>
-      <c r="T2" s="96" t="s">
+      <c r="U2" s="89"/>
+      <c r="V2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="96"/>
-      <c r="V2" s="96" t="s">
-        <v>9</v>
-      </c>
-      <c r="W2" s="96"/>
+      <c r="W2" s="89"/>
     </row>
     <row r="3" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="98" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="99" t="n">
+        <v>9</v>
+      </c>
+      <c r="B3" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="92" t="n">
         <v>79</v>
       </c>
-      <c r="D3" s="100" t="s">
+      <c r="D3" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="99" t="n">
+      <c r="E3" s="92" t="n">
         <v>143</v>
       </c>
-      <c r="F3" s="100" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="99" t="n">
+      <c r="F3" s="93" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="92" t="n">
         <v>79</v>
       </c>
-      <c r="H3" s="98" t="s">
+      <c r="H3" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="99" t="n">
+      <c r="I3" s="92" t="n">
         <v>143</v>
       </c>
-      <c r="J3" s="101"/>
-      <c r="K3" s="102"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="95"/>
       <c r="M3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="98" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="99" t="n">
+        <v>9</v>
+      </c>
+      <c r="N3" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="92" t="n">
         <v>79</v>
       </c>
-      <c r="P3" s="100" t="s">
+      <c r="P3" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="Q3" s="99" t="n">
+      <c r="Q3" s="92" t="n">
         <v>143</v>
       </c>
-      <c r="R3" s="100" t="s">
-        <v>41</v>
-      </c>
-      <c r="S3" s="99" t="n">
+      <c r="R3" s="93" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="92" t="n">
         <v>79</v>
       </c>
-      <c r="T3" s="98" t="s">
+      <c r="T3" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="U3" s="99" t="n">
+      <c r="U3" s="92" t="n">
         <v>143</v>
       </c>
-      <c r="V3" s="101"/>
-      <c r="W3" s="102"/>
+      <c r="V3" s="94"/>
+      <c r="W3" s="95"/>
     </row>
     <row r="4" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="103" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="104" t="n">
+      <c r="C4" s="97" t="n">
         <v>49</v>
       </c>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="99" t="n">
+      <c r="E4" s="92" t="n">
         <v>112</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="98" t="s">
+      <c r="F4" s="94"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="99" t="n">
+      <c r="I4" s="92" t="n">
         <v>56</v>
       </c>
-      <c r="J4" s="98" t="s">
+      <c r="J4" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="99" t="n">
+      <c r="K4" s="92" t="n">
         <v>96</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="105"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="98" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="98"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="Q4" s="99" t="n">
+      <c r="Q4" s="92" t="n">
         <v>112</v>
       </c>
-      <c r="R4" s="101"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="98" t="s">
+      <c r="R4" s="94"/>
+      <c r="S4" s="95"/>
+      <c r="T4" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="U4" s="99" t="n">
+      <c r="U4" s="92" t="n">
         <v>56</v>
       </c>
-      <c r="V4" s="98" t="s">
+      <c r="V4" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="W4" s="99" t="n">
+      <c r="W4" s="92" t="n">
         <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="96"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="99" t="n">
+      <c r="E5" s="92" t="n">
         <v>107</v>
       </c>
-      <c r="F5" s="98" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="99" t="n">
+      <c r="F5" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="92" t="n">
         <v>98</v>
       </c>
-      <c r="H5" s="98" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="99" t="n">
+      <c r="H5" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="92" t="n">
         <v>139</v>
       </c>
-      <c r="J5" s="98" t="s">
+      <c r="J5" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="99" t="n">
+      <c r="K5" s="92" t="n">
         <v>84</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="107"/>
-      <c r="O5" s="108"/>
-      <c r="P5" s="98" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="100"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="Q5" s="99" t="n">
+      <c r="Q5" s="92" t="n">
         <v>107</v>
       </c>
-      <c r="R5" s="98" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" s="99" t="n">
+      <c r="R5" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="92" t="n">
         <v>98</v>
       </c>
-      <c r="T5" s="98" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" s="99" t="n">
+      <c r="T5" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="U5" s="92" t="n">
         <v>139</v>
       </c>
-      <c r="V5" s="98" t="s">
+      <c r="V5" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="W5" s="99" t="n">
+      <c r="W5" s="92" t="n">
         <v>84</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="98" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="99" t="n">
+        <v>19</v>
+      </c>
+      <c r="B6" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="92" t="n">
         <v>98</v>
       </c>
-      <c r="D6" s="98" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="99" t="n">
+      <c r="D6" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="92" t="n">
         <v>139</v>
       </c>
-      <c r="F6" s="98" t="s">
+      <c r="F6" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="99" t="n">
+      <c r="G6" s="92" t="n">
         <v>74</v>
       </c>
-      <c r="H6" s="98" t="s">
+      <c r="H6" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="99" t="n">
+      <c r="I6" s="92" t="n">
         <v>107</v>
       </c>
-      <c r="J6" s="101"/>
-      <c r="K6" s="102"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="95"/>
       <c r="M6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="98" t="s">
-        <v>37</v>
-      </c>
-      <c r="O6" s="99" t="n">
+        <v>19</v>
+      </c>
+      <c r="N6" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="92" t="n">
         <v>98</v>
       </c>
-      <c r="P6" s="98" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q6" s="99" t="n">
+      <c r="P6" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="92" t="n">
         <v>139</v>
       </c>
-      <c r="R6" s="98" t="s">
+      <c r="R6" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="S6" s="99" t="n">
+      <c r="S6" s="92" t="n">
         <v>74</v>
       </c>
-      <c r="T6" s="98" t="s">
+      <c r="T6" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="U6" s="99" t="n">
+      <c r="U6" s="92" t="n">
         <v>107</v>
       </c>
-      <c r="V6" s="101"/>
-      <c r="W6" s="102"/>
+      <c r="V6" s="94"/>
+      <c r="W6" s="95"/>
     </row>
     <row r="7" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="98" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="109" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="98" t="s">
+      <c r="C7" s="102" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="99" t="n">
+      <c r="E7" s="92" t="n">
         <v>103</v>
       </c>
-      <c r="F7" s="101"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="98" t="s">
+      <c r="F7" s="94"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="99" t="n">
+      <c r="I7" s="92" t="n">
         <v>113</v>
       </c>
-      <c r="J7" s="98" t="s">
+      <c r="J7" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="99" t="n">
+      <c r="K7" s="92" t="n">
         <v>103</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="101"/>
-      <c r="O7" s="102"/>
-      <c r="P7" s="98" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="94"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="99" t="n">
+      <c r="Q7" s="92" t="n">
         <v>103</v>
       </c>
-      <c r="R7" s="101"/>
-      <c r="S7" s="102"/>
-      <c r="T7" s="98" t="s">
+      <c r="R7" s="94"/>
+      <c r="S7" s="95"/>
+      <c r="T7" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="U7" s="99" t="n">
+      <c r="U7" s="92" t="n">
         <v>113</v>
       </c>
-      <c r="V7" s="98" t="s">
+      <c r="V7" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="W7" s="99" t="n">
+      <c r="W7" s="92" t="n">
         <v>103</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="98" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="99" t="n">
+      <c r="C8" s="92" t="n">
         <v>66</v>
       </c>
-      <c r="D8" s="98" t="s">
+      <c r="D8" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="99" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="101"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="98" t="s">
+      <c r="E8" s="92" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="94"/>
+      <c r="G8" s="95"/>
+      <c r="H8" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="99" t="n">
+      <c r="I8" s="92" t="n">
         <v>83</v>
       </c>
-      <c r="J8" s="98" t="s">
+      <c r="J8" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="K8" s="99" t="n">
+      <c r="K8" s="92" t="n">
         <v>113</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N8" s="98" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="O8" s="99" t="n">
+      <c r="O8" s="92" t="n">
         <v>66</v>
       </c>
-      <c r="P8" s="98" t="s">
+      <c r="P8" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="Q8" s="99" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="101"/>
-      <c r="S8" s="102"/>
-      <c r="T8" s="98" t="s">
+      <c r="Q8" s="92" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="94"/>
+      <c r="S8" s="95"/>
+      <c r="T8" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="U8" s="99" t="n">
+      <c r="U8" s="92" t="n">
         <v>83</v>
       </c>
-      <c r="V8" s="98" t="s">
+      <c r="V8" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="W8" s="99" t="n">
+      <c r="W8" s="92" t="n">
         <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="98" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="99" t="n">
+      <c r="C9" s="92" t="n">
         <v>19</v>
       </c>
-      <c r="D9" s="98" t="s">
+      <c r="D9" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="99" t="n">
+      <c r="E9" s="92" t="n">
         <v>108</v>
       </c>
-      <c r="F9" s="98" t="s">
+      <c r="F9" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="99" t="n">
+      <c r="G9" s="92" t="n">
         <v>84</v>
       </c>
-      <c r="H9" s="101"/>
-      <c r="I9" s="102"/>
-      <c r="J9" s="98" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="99" t="n">
+      <c r="H9" s="94"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="92" t="n">
         <v>38</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" s="98" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="99" t="n">
+      <c r="O9" s="92" t="n">
         <v>19</v>
       </c>
-      <c r="P9" s="98" t="s">
+      <c r="P9" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="Q9" s="99" t="n">
+      <c r="Q9" s="92" t="n">
         <v>108</v>
       </c>
-      <c r="R9" s="98" t="s">
+      <c r="R9" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="S9" s="99" t="n">
+      <c r="S9" s="92" t="n">
         <v>84</v>
       </c>
-      <c r="T9" s="101"/>
-      <c r="U9" s="102"/>
-      <c r="V9" s="98" t="s">
-        <v>12</v>
-      </c>
-      <c r="W9" s="99" t="n">
+      <c r="T9" s="94"/>
+      <c r="U9" s="95"/>
+      <c r="V9" s="91" t="s">
+        <v>11</v>
+      </c>
+      <c r="W9" s="92" t="n">
         <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="102"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="98" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="94"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="95"/>
+      <c r="H10" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="99" t="n">
+      <c r="I10" s="92" t="n">
         <v>108</v>
       </c>
-      <c r="J10" s="101"/>
-      <c r="K10" s="102"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="95"/>
       <c r="M10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="101"/>
-      <c r="O10" s="102"/>
-      <c r="P10" s="101"/>
-      <c r="Q10" s="102"/>
-      <c r="R10" s="101"/>
-      <c r="S10" s="102"/>
-      <c r="T10" s="98" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="94"/>
+      <c r="O10" s="95"/>
+      <c r="P10" s="94"/>
+      <c r="Q10" s="95"/>
+      <c r="R10" s="94"/>
+      <c r="S10" s="95"/>
+      <c r="T10" s="91" t="s">
         <v>64</v>
       </c>
-      <c r="U10" s="99" t="n">
+      <c r="U10" s="92" t="n">
         <v>108</v>
       </c>
-      <c r="V10" s="101"/>
-      <c r="W10" s="102"/>
+      <c r="V10" s="94"/>
+      <c r="W10" s="95"/>
     </row>
     <row r="11" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="101"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="102"/>
-      <c r="L11" s="42"/>
+        <v>32</v>
+      </c>
+      <c r="B11" s="94"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="95"/>
+      <c r="J11" s="94"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="77"/>
       <c r="M11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="101"/>
-      <c r="O11" s="102"/>
-      <c r="P11" s="101"/>
-      <c r="Q11" s="102"/>
-      <c r="R11" s="101"/>
-      <c r="S11" s="102"/>
-      <c r="T11" s="101"/>
-      <c r="U11" s="102"/>
-      <c r="V11" s="101"/>
-      <c r="W11" s="102"/>
+        <v>32</v>
+      </c>
+      <c r="N11" s="94"/>
+      <c r="O11" s="95"/>
+      <c r="P11" s="94"/>
+      <c r="Q11" s="95"/>
+      <c r="R11" s="94"/>
+      <c r="S11" s="95"/>
+      <c r="T11" s="94"/>
+      <c r="U11" s="95"/>
+      <c r="V11" s="94"/>
+      <c r="W11" s="95"/>
     </row>
     <row r="13" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="45"/>
+      <c r="B13" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="80"/>
+      <c r="R13" s="80"/>
+      <c r="S13" s="80"/>
+      <c r="T13" s="80"/>
+      <c r="U13" s="80"/>
+      <c r="V13" s="80"/>
     </row>
     <row r="14" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="48"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="48"/>
+      <c r="B14" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="82"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="83"/>
+      <c r="N14" s="83"/>
+      <c r="O14" s="83"/>
+      <c r="P14" s="83"/>
+      <c r="Q14" s="83"/>
+      <c r="R14" s="83"/>
+      <c r="S14" s="83"/>
+      <c r="T14" s="83"/>
+      <c r="U14" s="83"/>
+      <c r="V14" s="83"/>
+      <c r="W14" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -3778,44 +3353,44 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="F1" s="111" t="s">
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="F1" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="110" t="s">
+      <c r="G1" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="105" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="113" t="s">
+      <c r="F2" s="106" t="s">
         <v>69</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>47</v>
@@ -3823,7 +3398,7 @@
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>29</v>
@@ -3834,8 +3409,8 @@
       <c r="D3" s="7" t="n">
         <v>79</v>
       </c>
-      <c r="F3" s="114" t="s">
-        <v>10</v>
+      <c r="F3" s="107" t="s">
+        <v>9</v>
       </c>
       <c r="G3" s="7" t="n">
         <v>29</v>
@@ -3849,7 +3424,7 @@
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>53</v>
@@ -3860,8 +3435,8 @@
       <c r="D4" s="7" t="n">
         <v>49</v>
       </c>
-      <c r="F4" s="114" t="s">
-        <v>13</v>
+      <c r="F4" s="107" t="s">
+        <v>12</v>
       </c>
       <c r="G4" s="7" t="n">
         <v>53</v>
@@ -3875,7 +3450,7 @@
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>0</v>
@@ -3886,8 +3461,8 @@
       <c r="D5" s="7" t="n">
         <v>49</v>
       </c>
-      <c r="F5" s="114" t="s">
-        <v>16</v>
+      <c r="F5" s="107" t="s">
+        <v>15</v>
       </c>
       <c r="G5" s="7" t="n">
         <v>0</v>
@@ -3901,7 +3476,7 @@
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>22</v>
@@ -3912,8 +3487,8 @@
       <c r="D6" s="7" t="n">
         <v>98</v>
       </c>
-      <c r="F6" s="114" t="s">
-        <v>20</v>
+      <c r="F6" s="107" t="s">
+        <v>19</v>
       </c>
       <c r="G6" s="7" t="n">
         <v>22</v>
@@ -3927,7 +3502,7 @@
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>60</v>
@@ -3935,11 +3510,11 @@
       <c r="C7" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="D7" s="115" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="114" t="s">
-        <v>22</v>
+      <c r="D7" s="108" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="107" t="s">
+        <v>21</v>
       </c>
       <c r="G7" s="7" t="n">
         <v>60</v>
@@ -3953,7 +3528,7 @@
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>18</v>
@@ -3964,8 +3539,8 @@
       <c r="D8" s="7" t="n">
         <v>66</v>
       </c>
-      <c r="F8" s="114" t="s">
-        <v>27</v>
+      <c r="F8" s="107" t="s">
+        <v>26</v>
       </c>
       <c r="G8" s="7" t="n">
         <v>18</v>
@@ -3979,7 +3554,7 @@
     </row>
     <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>0</v>
@@ -3990,8 +3565,8 @@
       <c r="D9" s="7" t="n">
         <v>19</v>
       </c>
-      <c r="F9" s="114" t="s">
-        <v>29</v>
+      <c r="F9" s="107" t="s">
+        <v>28</v>
       </c>
       <c r="G9" s="7" t="n">
         <v>0</v>
@@ -4005,7 +3580,7 @@
     </row>
     <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>53</v>
@@ -4016,8 +3591,8 @@
       <c r="D10" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="114" t="s">
-        <v>32</v>
+      <c r="F10" s="107" t="s">
+        <v>31</v>
       </c>
       <c r="G10" s="7" t="n">
         <v>53</v>
@@ -4031,7 +3606,7 @@
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>53</v>
@@ -4042,8 +3617,8 @@
       <c r="D11" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="114" t="s">
-        <v>33</v>
+      <c r="F11" s="107" t="s">
+        <v>32</v>
       </c>
       <c r="G11" s="7" t="n">
         <v>53</v>
@@ -4056,29 +3631,29 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F12" s="116"/>
+      <c r="F12" s="109"/>
     </row>
     <row r="13" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="105" t="s">
         <v>70</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="113" t="s">
+      <c r="F13" s="106" t="s">
         <v>71</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>47</v>
@@ -4086,7 +3661,7 @@
     </row>
     <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="7" t="n">
         <v>0</v>
@@ -4097,8 +3672,8 @@
       <c r="D14" s="7" t="n">
         <v>143</v>
       </c>
-      <c r="F14" s="114" t="s">
-        <v>10</v>
+      <c r="F14" s="107" t="s">
+        <v>9</v>
       </c>
       <c r="G14" s="7" t="n">
         <v>0</v>
@@ -4112,7 +3687,7 @@
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="7" t="n">
         <v>45</v>
@@ -4123,8 +3698,8 @@
       <c r="D15" s="7" t="n">
         <v>112</v>
       </c>
-      <c r="F15" s="114" t="s">
-        <v>13</v>
+      <c r="F15" s="107" t="s">
+        <v>12</v>
       </c>
       <c r="G15" s="7" t="n">
         <v>45</v>
@@ -4138,7 +3713,7 @@
     </row>
     <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>18</v>
@@ -4149,8 +3724,8 @@
       <c r="D16" s="7" t="n">
         <v>107</v>
       </c>
-      <c r="F16" s="114" t="s">
-        <v>16</v>
+      <c r="F16" s="107" t="s">
+        <v>15</v>
       </c>
       <c r="G16" s="7" t="n">
         <v>18</v>
@@ -4164,7 +3739,7 @@
     </row>
     <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="7" t="n">
         <v>27</v>
@@ -4175,8 +3750,8 @@
       <c r="D17" s="7" t="n">
         <v>139</v>
       </c>
-      <c r="F17" s="114" t="s">
-        <v>20</v>
+      <c r="F17" s="107" t="s">
+        <v>19</v>
       </c>
       <c r="G17" s="7" t="n">
         <v>27</v>
@@ -4190,25 +3765,25 @@
     </row>
     <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C18" s="115" t="s">
-        <v>45</v>
+      <c r="C18" s="108" t="s">
+        <v>43</v>
       </c>
       <c r="D18" s="7" t="n">
         <v>103</v>
       </c>
-      <c r="F18" s="114" t="s">
-        <v>22</v>
+      <c r="F18" s="107" t="s">
+        <v>21</v>
       </c>
       <c r="G18" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="H18" s="115" t="s">
-        <v>45</v>
+      <c r="H18" s="108" t="s">
+        <v>43</v>
       </c>
       <c r="I18" s="7" t="n">
         <v>103</v>
@@ -4216,7 +3791,7 @@
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="7" t="n">
         <v>42</v>
@@ -4227,8 +3802,8 @@
       <c r="D19" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="114" t="s">
-        <v>27</v>
+      <c r="F19" s="107" t="s">
+        <v>26</v>
       </c>
       <c r="G19" s="7" t="n">
         <v>42</v>
@@ -4242,7 +3817,7 @@
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="7" t="n">
         <v>42</v>
@@ -4253,8 +3828,8 @@
       <c r="D20" s="7" t="n">
         <v>108</v>
       </c>
-      <c r="F20" s="114" t="s">
-        <v>29</v>
+      <c r="F20" s="107" t="s">
+        <v>28</v>
       </c>
       <c r="G20" s="7" t="n">
         <v>42</v>
@@ -4268,7 +3843,7 @@
     </row>
     <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="7" t="n">
         <v>27</v>
@@ -4279,8 +3854,8 @@
       <c r="D21" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F21" s="114" t="s">
-        <v>32</v>
+      <c r="F21" s="107" t="s">
+        <v>31</v>
       </c>
       <c r="G21" s="7" t="n">
         <v>27</v>
@@ -4294,7 +3869,7 @@
     </row>
     <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="7" t="n">
         <v>27</v>
@@ -4305,8 +3880,8 @@
       <c r="D22" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="114" t="s">
-        <v>33</v>
+      <c r="F22" s="107" t="s">
+        <v>32</v>
       </c>
       <c r="G22" s="7" t="n">
         <v>27</v>
@@ -4319,29 +3894,29 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F23" s="116"/>
+      <c r="F23" s="109"/>
     </row>
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="112" t="s">
+      <c r="A24" s="105" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="113" t="s">
+      <c r="F24" s="106" t="s">
         <v>73</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>47</v>
@@ -4349,7 +3924,7 @@
     </row>
     <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="7" t="n">
         <v>29</v>
@@ -4360,8 +3935,8 @@
       <c r="D25" s="7" t="n">
         <v>79</v>
       </c>
-      <c r="F25" s="114" t="s">
-        <v>10</v>
+      <c r="F25" s="107" t="s">
+        <v>9</v>
       </c>
       <c r="G25" s="7" t="n">
         <v>29</v>
@@ -4375,7 +3950,7 @@
     </row>
     <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="7" t="n">
         <v>53</v>
@@ -4386,8 +3961,8 @@
       <c r="D26" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F26" s="114" t="s">
-        <v>13</v>
+      <c r="F26" s="107" t="s">
+        <v>12</v>
       </c>
       <c r="G26" s="7" t="n">
         <v>53</v>
@@ -4401,7 +3976,7 @@
     </row>
     <row r="27" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="7" t="n">
         <v>22</v>
@@ -4412,8 +3987,8 @@
       <c r="D27" s="7" t="n">
         <v>98</v>
       </c>
-      <c r="F27" s="114" t="s">
-        <v>16</v>
+      <c r="F27" s="107" t="s">
+        <v>15</v>
       </c>
       <c r="G27" s="7" t="n">
         <v>22</v>
@@ -4427,7 +4002,7 @@
     </row>
     <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="7" t="n">
         <v>60</v>
@@ -4438,8 +4013,8 @@
       <c r="D28" s="7" t="n">
         <v>74</v>
       </c>
-      <c r="F28" s="114" t="s">
-        <v>20</v>
+      <c r="F28" s="107" t="s">
+        <v>19</v>
       </c>
       <c r="G28" s="7" t="n">
         <v>60</v>
@@ -4453,7 +4028,7 @@
     </row>
     <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" s="7" t="n">
         <v>60</v>
@@ -4464,8 +4039,8 @@
       <c r="D29" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F29" s="114" t="s">
-        <v>22</v>
+      <c r="F29" s="107" t="s">
+        <v>21</v>
       </c>
       <c r="G29" s="7" t="n">
         <v>60</v>
@@ -4479,7 +4054,7 @@
     </row>
     <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="7" t="n">
         <v>38</v>
@@ -4490,8 +4065,8 @@
       <c r="D30" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F30" s="114" t="s">
-        <v>27</v>
+      <c r="F30" s="107" t="s">
+        <v>26</v>
       </c>
       <c r="G30" s="7" t="n">
         <v>38</v>
@@ -4505,7 +4080,7 @@
     </row>
     <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="7" t="n">
         <v>79</v>
@@ -4516,8 +4091,8 @@
       <c r="D31" s="7" t="n">
         <v>84</v>
       </c>
-      <c r="F31" s="114" t="s">
-        <v>29</v>
+      <c r="F31" s="107" t="s">
+        <v>28</v>
       </c>
       <c r="G31" s="7" t="n">
         <v>79</v>
@@ -4531,7 +4106,7 @@
     </row>
     <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="7" t="n">
         <v>22</v>
@@ -4542,8 +4117,8 @@
       <c r="D32" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F32" s="114" t="s">
-        <v>32</v>
+      <c r="F32" s="107" t="s">
+        <v>31</v>
       </c>
       <c r="G32" s="7" t="n">
         <v>22</v>
@@ -4557,7 +4132,7 @@
     </row>
     <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="7" t="n">
         <v>22</v>
@@ -4568,8 +4143,8 @@
       <c r="D33" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F33" s="114" t="s">
-        <v>33</v>
+      <c r="F33" s="107" t="s">
+        <v>32</v>
       </c>
       <c r="G33" s="7" t="n">
         <v>22</v>
@@ -4582,29 +4157,29 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F34" s="116"/>
+      <c r="F34" s="109"/>
     </row>
     <row r="35" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="112" t="s">
+      <c r="A35" s="105" t="s">
         <v>74</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="113" t="s">
+      <c r="F35" s="106" t="s">
         <v>75</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I35" s="7" t="s">
         <v>47</v>
@@ -4612,7 +4187,7 @@
     </row>
     <row r="36" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" s="7" t="n">
         <v>0</v>
@@ -4623,8 +4198,8 @@
       <c r="D36" s="7" t="n">
         <v>143</v>
       </c>
-      <c r="F36" s="114" t="s">
-        <v>10</v>
+      <c r="F36" s="107" t="s">
+        <v>9</v>
       </c>
       <c r="G36" s="7" t="n">
         <v>0</v>
@@ -4638,7 +4213,7 @@
     </row>
     <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B37" s="7" t="n">
         <v>45</v>
@@ -4649,8 +4224,8 @@
       <c r="D37" s="7" t="n">
         <v>56</v>
       </c>
-      <c r="F37" s="114" t="s">
-        <v>13</v>
+      <c r="F37" s="107" t="s">
+        <v>12</v>
       </c>
       <c r="G37" s="7" t="n">
         <v>45</v>
@@ -4664,7 +4239,7 @@
     </row>
     <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B38" s="7" t="n">
         <v>27</v>
@@ -4675,8 +4250,8 @@
       <c r="D38" s="7" t="n">
         <v>139</v>
       </c>
-      <c r="F38" s="114" t="s">
-        <v>16</v>
+      <c r="F38" s="107" t="s">
+        <v>15</v>
       </c>
       <c r="G38" s="7" t="n">
         <v>27</v>
@@ -4690,7 +4265,7 @@
     </row>
     <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B39" s="7" t="n">
         <v>18</v>
@@ -4701,8 +4276,8 @@
       <c r="D39" s="7" t="n">
         <v>107</v>
       </c>
-      <c r="F39" s="114" t="s">
-        <v>20</v>
+      <c r="F39" s="107" t="s">
+        <v>19</v>
       </c>
       <c r="G39" s="7" t="n">
         <v>18</v>
@@ -4716,25 +4291,25 @@
     </row>
     <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B40" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C40" s="115" t="s">
-        <v>45</v>
+      <c r="C40" s="108" t="s">
+        <v>43</v>
       </c>
       <c r="D40" s="7" t="n">
         <v>113</v>
       </c>
-      <c r="F40" s="114" t="s">
-        <v>22</v>
+      <c r="F40" s="107" t="s">
+        <v>21</v>
       </c>
       <c r="G40" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="H40" s="115" t="s">
-        <v>45</v>
+      <c r="H40" s="108" t="s">
+        <v>43</v>
       </c>
       <c r="I40" s="7" t="n">
         <v>113</v>
@@ -4742,7 +4317,7 @@
     </row>
     <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B41" s="7" t="n">
         <v>42</v>
@@ -4753,8 +4328,8 @@
       <c r="D41" s="7" t="n">
         <v>83</v>
       </c>
-      <c r="F41" s="114" t="s">
-        <v>27</v>
+      <c r="F41" s="107" t="s">
+        <v>26</v>
       </c>
       <c r="G41" s="7" t="n">
         <v>42</v>
@@ -4768,7 +4343,7 @@
     </row>
     <row r="42" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B42" s="7" t="n">
         <v>60</v>
@@ -4779,8 +4354,8 @@
       <c r="D42" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F42" s="114" t="s">
-        <v>29</v>
+      <c r="F42" s="107" t="s">
+        <v>28</v>
       </c>
       <c r="G42" s="7" t="n">
         <v>60</v>
@@ -4794,7 +4369,7 @@
     </row>
     <row r="43" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B43" s="7" t="n">
         <v>0</v>
@@ -4805,8 +4380,8 @@
       <c r="D43" s="7" t="n">
         <v>108</v>
       </c>
-      <c r="F43" s="114" t="s">
-        <v>32</v>
+      <c r="F43" s="107" t="s">
+        <v>31</v>
       </c>
       <c r="G43" s="7" t="n">
         <v>60</v>
@@ -4820,55 +4395,55 @@
     </row>
     <row r="44" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="107" t="s">
+        <v>32</v>
+      </c>
+      <c r="G44" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D45" s="77"/>
+      <c r="F45" s="109"/>
+    </row>
+    <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="105" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="B44" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C44" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="114" t="s">
-        <v>33</v>
-      </c>
-      <c r="G44" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D45" s="42"/>
-      <c r="F45" s="116"/>
-    </row>
-    <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="112" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F46" s="113" t="s">
+      <c r="F46" s="106" t="s">
         <v>77</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>47</v>
@@ -4876,7 +4451,7 @@
     </row>
     <row r="47" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" s="7" t="n">
         <v>38</v>
@@ -4887,8 +4462,8 @@
       <c r="D47" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F47" s="114" t="s">
-        <v>10</v>
+      <c r="F47" s="107" t="s">
+        <v>9</v>
       </c>
       <c r="G47" s="7" t="n">
         <v>38</v>
@@ -4902,7 +4477,7 @@
     </row>
     <row r="48" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B48" s="7" t="n">
         <v>0</v>
@@ -4913,8 +4488,8 @@
       <c r="D48" s="7" t="n">
         <v>96</v>
       </c>
-      <c r="F48" s="114" t="s">
-        <v>13</v>
+      <c r="F48" s="107" t="s">
+        <v>12</v>
       </c>
       <c r="G48" s="7" t="n">
         <v>0</v>
@@ -4928,7 +4503,7 @@
     </row>
     <row r="49" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B49" s="7" t="n">
         <v>29</v>
@@ -4939,8 +4514,8 @@
       <c r="D49" s="7" t="n">
         <v>84</v>
       </c>
-      <c r="F49" s="114" t="s">
-        <v>16</v>
+      <c r="F49" s="107" t="s">
+        <v>15</v>
       </c>
       <c r="G49" s="7" t="n">
         <v>29</v>
@@ -4954,7 +4529,7 @@
     </row>
     <row r="50" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="7" t="n">
         <v>0</v>
@@ -4965,8 +4540,8 @@
       <c r="D50" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F50" s="114" t="s">
-        <v>20</v>
+      <c r="F50" s="107" t="s">
+        <v>19</v>
       </c>
       <c r="G50" s="7" t="n">
         <v>29</v>
@@ -4980,7 +4555,7 @@
     </row>
     <row r="51" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B51" s="7" t="n">
         <v>51</v>
@@ -4991,8 +4566,8 @@
       <c r="D51" s="7" t="n">
         <v>103</v>
       </c>
-      <c r="F51" s="114" t="s">
-        <v>22</v>
+      <c r="F51" s="107" t="s">
+        <v>21</v>
       </c>
       <c r="G51" s="7" t="n">
         <v>51</v>
@@ -5006,7 +4581,7 @@
     </row>
     <row r="52" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B52" s="7" t="n">
         <v>42</v>
@@ -5017,8 +4592,8 @@
       <c r="D52" s="7" t="n">
         <v>113</v>
       </c>
-      <c r="F52" s="114" t="s">
-        <v>27</v>
+      <c r="F52" s="107" t="s">
+        <v>26</v>
       </c>
       <c r="G52" s="7" t="n">
         <v>42</v>
@@ -5032,7 +4607,7 @@
     </row>
     <row r="53" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B53" s="7" t="n">
         <v>0</v>
@@ -5043,8 +4618,8 @@
       <c r="D53" s="7" t="n">
         <v>38</v>
       </c>
-      <c r="F53" s="114" t="s">
-        <v>29</v>
+      <c r="F53" s="107" t="s">
+        <v>28</v>
       </c>
       <c r="G53" s="7" t="n">
         <v>0</v>
@@ -5058,7 +4633,7 @@
     </row>
     <row r="54" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" s="7" t="n">
         <v>0</v>
@@ -5069,8 +4644,8 @@
       <c r="D54" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F54" s="114" t="s">
-        <v>32</v>
+      <c r="F54" s="107" t="s">
+        <v>31</v>
       </c>
       <c r="G54" s="7" t="n">
         <v>0</v>
@@ -5084,7 +4659,7 @@
     </row>
     <row r="55" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B55" s="7" t="n">
         <v>0</v>
@@ -5095,8 +4670,8 @@
       <c r="D55" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F55" s="114" t="s">
-        <v>33</v>
+      <c r="F55" s="107" t="s">
+        <v>32</v>
       </c>
       <c r="G55" s="7" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Removed print statemeents form two files and added db password
</commit_message>
<xml_diff>
--- a/data_cleaning/1.test_data/B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/data_cleaning/1.test_data/B0.02 B0.03 B0.04 Timetable.xlsx
@@ -928,9 +928,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="111">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -1266,12 +1266,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="3" name="Comma" xfId="0"/>
-    <cellStyle builtinId="5" name="Percent" xfId="1"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="2"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
-    <cellStyle builtinId="4" name="Currency" xfId="4"/>
-    <cellStyle builtinId="0" name="Normal" xfId="5"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="0"/>
+    <cellStyle builtinId="4" name="Currency" xfId="1"/>
+    <cellStyle builtinId="5" name="Percent" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="3" name="Comma" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>

</xml_diff>